<commit_message>
Updated with Occupancy and Nightly Rate stats
</commit_message>
<xml_diff>
--- a/Envelope Math.xlsx
+++ b/Envelope Math.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25725"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-20" windowWidth="28800" windowHeight="17460" tabRatio="500" firstSheet="14" activeTab="14"/>
+    <workbookView xWindow="0" yWindow="-20" windowWidth="28800" windowHeight="17460" tabRatio="500" firstSheet="5" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="January" sheetId="3" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1413" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1440" uniqueCount="80">
   <si>
     <t>maybe extra 71</t>
   </si>
@@ -394,7 +394,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1086">
+  <cellStyleXfs count="1104">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -427,6 +427,24 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1524,7 +1542,7 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1086">
+  <cellStyles count="1104">
     <cellStyle name="Currency" xfId="31" builtinId="4"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -2068,6 +2086,15 @@
     <cellStyle name="Followed Hyperlink" xfId="1081" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="1083" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="1085" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1087" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1089" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1091" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1093" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1095" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1097" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1099" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1101" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1103" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -2610,6 +2637,15 @@
     <cellStyle name="Hyperlink" xfId="1080" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1082" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1084" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1086" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1088" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1090" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1092" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1094" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1096" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1098" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1100" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1102" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="174">
@@ -5990,10 +6026,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:U48"/>
+  <dimension ref="B1:U48"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A2" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="P45" sqref="P45"/>
+    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6005,6 +6041,14 @@
     <col min="12" max="12" width="12.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="2:21">
+      <c r="G1" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="K1" s="19" t="s">
+        <v>46</v>
+      </c>
+    </row>
     <row r="2" spans="2:21" ht="25">
       <c r="B2" s="4" t="s">
         <v>32</v>
@@ -6013,10 +6057,21 @@
         <f>D48+L48</f>
         <v>4904.4500000000007</v>
       </c>
-      <c r="F2" t="s">
-        <v>35</v>
+      <c r="G2" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="I2" s="17">
+        <f>COUNTIF(D12:D42,"Y")/COUNT(C12:C42)</f>
+        <v>0.87096774193548387</v>
       </c>
       <c r="J2" s="1"/>
+      <c r="K2" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="M2" s="17">
+        <f>COUNTIF(L12:L42,"Y")/COUNT(K12:K42)</f>
+        <v>0.90322580645161288</v>
+      </c>
     </row>
     <row r="3" spans="2:21" ht="25">
       <c r="B3" s="4" t="s">
@@ -6026,10 +6081,21 @@
         <f>C48+K48</f>
         <v>5704.7000000000007</v>
       </c>
-      <c r="F3" t="s">
-        <v>36</v>
+      <c r="G3" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="I3" s="18">
+        <f>AVERAGE(C12:C42)</f>
+        <v>142.58064516129033</v>
       </c>
       <c r="J3" s="1"/>
+      <c r="K3" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="M3" s="18">
+        <f>AVERAGE(K12:K42)</f>
+        <v>212.58064516129033</v>
+      </c>
     </row>
     <row r="4" spans="2:21" ht="25">
       <c r="B4" s="4" t="s">
@@ -6039,16 +6105,20 @@
         <f ca="1">D3-E44-M44</f>
         <v>4879.7000000000007</v>
       </c>
+      <c r="G4" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="I4" s="18">
+        <f>I3*I2</f>
+        <v>124.18314255983351</v>
+      </c>
       <c r="J4" s="1"/>
-    </row>
-    <row r="6" spans="2:21">
-      <c r="F6" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="7" spans="2:21">
-      <c r="F7" t="s">
-        <v>38</v>
+      <c r="K4" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="M4" s="18">
+        <f>M3*M2</f>
+        <v>192.00832466181063</v>
       </c>
     </row>
     <row r="9" spans="2:21" ht="25">
@@ -10780,10 +10850,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:U48"/>
+  <dimension ref="B1:U48"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -10795,6 +10865,14 @@
     <col min="12" max="12" width="12.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="2:21">
+      <c r="G1" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="K1" s="19" t="s">
+        <v>46</v>
+      </c>
+    </row>
     <row r="2" spans="2:21" ht="25">
       <c r="B2" s="4" t="s">
         <v>32</v>
@@ -10803,10 +10881,21 @@
         <f>D48+L48</f>
         <v>863.43000000000006</v>
       </c>
-      <c r="F2" t="s">
-        <v>35</v>
+      <c r="G2" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="I2" s="17">
+        <f>COUNTIF(D12:D42,"Y")/COUNT(C12:C42)</f>
+        <v>0.67741935483870963</v>
       </c>
       <c r="J2" s="1"/>
+      <c r="K2" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="M2" s="17">
+        <f>COUNTIF(L12:L42,"Y")/COUNT(K12:K42)</f>
+        <v>0.58064516129032262</v>
+      </c>
     </row>
     <row r="3" spans="2:21" ht="25">
       <c r="B3" s="4" t="s">
@@ -10816,10 +10905,21 @@
         <f>C48+K48</f>
         <v>3196.2799999999997</v>
       </c>
-      <c r="F3" t="s">
-        <v>36</v>
+      <c r="G3" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="I3" s="18">
+        <f>AVERAGE(C12:C42)</f>
+        <v>115.7741935483871</v>
       </c>
       <c r="J3" s="1"/>
+      <c r="K3" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="M3" s="18">
+        <f>AVERAGE(K12:K42)</f>
+        <v>155.96774193548387</v>
+      </c>
     </row>
     <row r="4" spans="2:21" ht="25">
       <c r="B4" s="4" t="s">
@@ -10829,16 +10929,20 @@
         <f ca="1">D3-E44-M44</f>
         <v>1551.2799999999997</v>
       </c>
+      <c r="G4" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="I4" s="18">
+        <f>I3*I2</f>
+        <v>78.427679500520284</v>
+      </c>
       <c r="J4" s="1"/>
-    </row>
-    <row r="6" spans="2:21">
-      <c r="F6" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="7" spans="2:21">
-      <c r="F7" t="s">
-        <v>38</v>
+      <c r="K4" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="M4" s="18">
+        <f>M3*M2</f>
+        <v>90.561914672216446</v>
       </c>
     </row>
     <row r="9" spans="2:21" ht="25">
@@ -17855,10 +17959,10 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:U47"/>
+  <dimension ref="B1:U47"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12:C41"/>
+      <selection activeCell="F1" sqref="F1:F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -17870,6 +17974,14 @@
     <col min="12" max="12" width="12.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="2:21">
+      <c r="G1" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="K1" s="19" t="s">
+        <v>46</v>
+      </c>
+    </row>
     <row r="2" spans="2:21" ht="25">
       <c r="B2" s="4" t="s">
         <v>32</v>
@@ -17878,10 +17990,21 @@
         <f>D47+L47</f>
         <v>269.78999999999996</v>
       </c>
-      <c r="F2" t="s">
-        <v>35</v>
+      <c r="G2" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="I2" s="17">
+        <f>COUNTIF(D12:D41,"Y")/COUNT(C12:C41)</f>
+        <v>0.7</v>
       </c>
       <c r="J2" s="1"/>
+      <c r="K2" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="M2" s="17">
+        <f>COUNTIF(L12:L41,"Y")/COUNT(K12:K41)</f>
+        <v>0.36666666666666664</v>
+      </c>
     </row>
     <row r="3" spans="2:21" ht="25">
       <c r="B3" s="4" t="s">
@@ -17891,10 +18014,21 @@
         <f>C47+K47</f>
         <v>5493.24</v>
       </c>
-      <c r="F3" t="s">
-        <v>36</v>
+      <c r="G3" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="I3" s="18">
+        <f>AVERAGE(C12:C41)</f>
+        <v>140.4</v>
       </c>
       <c r="J3" s="1"/>
+      <c r="K3" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="M3" s="18">
+        <f>AVERAGE(K12:K41)</f>
+        <v>219.33333333333334</v>
+      </c>
     </row>
     <row r="4" spans="2:21" ht="25">
       <c r="B4" s="4" t="s">
@@ -17904,16 +18038,20 @@
         <f ca="1">D3-E43-M43</f>
         <v>568.23999999999978</v>
       </c>
+      <c r="G4" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="I4" s="18">
+        <f>I3*I2</f>
+        <v>98.28</v>
+      </c>
       <c r="J4" s="1"/>
-    </row>
-    <row r="6" spans="2:21">
-      <c r="F6" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="7" spans="2:21">
-      <c r="F7" t="s">
-        <v>38</v>
+      <c r="K4" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="M4" s="18">
+        <f>M3*M2</f>
+        <v>80.422222222222217</v>
       </c>
     </row>
     <row r="9" spans="2:21" ht="25">
@@ -19499,7 +19637,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R71"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
@@ -21619,10 +21757,10 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:U48"/>
+  <dimension ref="B1:U48"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A2" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -21634,6 +21772,14 @@
     <col min="12" max="12" width="12.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="2:21">
+      <c r="G1" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="K1" s="19" t="s">
+        <v>46</v>
+      </c>
+    </row>
     <row r="2" spans="2:21" ht="25">
       <c r="B2" s="4" t="s">
         <v>32</v>
@@ -21642,10 +21788,21 @@
         <f>D48+L48</f>
         <v>-4590.88</v>
       </c>
-      <c r="F2" t="s">
-        <v>35</v>
+      <c r="G2" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="I2" s="17">
+        <f>COUNTIF(D12:D42,"Y")/COUNT(C12:C42)</f>
+        <v>0.12903225806451613</v>
       </c>
       <c r="J2" s="1"/>
+      <c r="K2" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="M2" s="17">
+        <f>COUNTIF(L12:L42,"Y")/COUNT(K12:K42)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="3" spans="2:21" ht="25">
       <c r="B3" s="4" t="s">
@@ -21655,10 +21812,21 @@
         <f>C48+K48</f>
         <v>6091.73</v>
       </c>
-      <c r="F3" t="s">
-        <v>36</v>
+      <c r="G3" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="I3" s="18">
+        <f>AVERAGE(C12:C42)</f>
+        <v>143.12903225806451</v>
       </c>
       <c r="J3" s="1"/>
+      <c r="K3" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="M3" s="18">
+        <f>AVERAGE(K12:K42)</f>
+        <v>224.90322580645162</v>
+      </c>
     </row>
     <row r="4" spans="2:21" ht="25">
       <c r="B4" s="4" t="s">
@@ -21668,16 +21836,20 @@
         <f ca="1">D3-E44-M44</f>
         <v>-2560.2700000000004</v>
       </c>
+      <c r="G4" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="I4" s="18">
+        <f>I3*I2</f>
+        <v>18.468262226847035</v>
+      </c>
       <c r="J4" s="1"/>
-    </row>
-    <row r="6" spans="2:21">
-      <c r="F6" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="7" spans="2:21">
-      <c r="F7" t="s">
-        <v>38</v>
+      <c r="K4" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="M4" s="18">
+        <f>M3*M2</f>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="2:21" ht="25">
@@ -24901,10 +25073,10 @@
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:U47"/>
+  <dimension ref="B1:U47"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -24916,6 +25088,14 @@
     <col min="12" max="12" width="12.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="2:21">
+      <c r="G1" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="K1" s="19" t="s">
+        <v>46</v>
+      </c>
+    </row>
     <row r="2" spans="2:21" ht="25">
       <c r="B2" s="4" t="s">
         <v>32</v>
@@ -24924,10 +25104,21 @@
         <f>D47+L47</f>
         <v>-4975</v>
       </c>
-      <c r="F2" t="s">
-        <v>35</v>
+      <c r="G2" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="I2" s="17">
+        <f>COUNTIF(D12:D41,"Y")/COUNT(C12:C41)</f>
+        <v>0</v>
       </c>
       <c r="J2" s="1"/>
+      <c r="K2" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="M2" s="17">
+        <f>COUNTIF(L12:L41,"Y")/COUNT(K12:K41)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="3" spans="2:21" ht="25">
       <c r="B3" s="4" t="s">
@@ -24937,10 +25128,21 @@
         <f>C47+K47</f>
         <v>4105.17</v>
       </c>
-      <c r="F3" t="s">
-        <v>36</v>
+      <c r="G3" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="I3" s="18">
+        <f>AVERAGE(C12:C41)</f>
+        <v>124.33333333333333</v>
       </c>
       <c r="J3" s="1"/>
+      <c r="K3" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="M3" s="18">
+        <f>AVERAGE(K12:K41)</f>
+        <v>187.7</v>
+      </c>
     </row>
     <row r="4" spans="2:21" ht="25">
       <c r="B4" s="4" t="s">
@@ -24950,16 +25152,20 @@
         <f ca="1">D3-E43-M43</f>
         <v>-3327.83</v>
       </c>
+      <c r="G4" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="I4" s="18">
+        <f>I3*I2</f>
+        <v>0</v>
+      </c>
       <c r="J4" s="1"/>
-    </row>
-    <row r="6" spans="2:21">
-      <c r="F6" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="7" spans="2:21">
-      <c r="F7" t="s">
-        <v>38</v>
+      <c r="K4" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="M4" s="18">
+        <f>M3*M2</f>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="2:21" ht="25">
@@ -32871,7 +33077,7 @@
   <dimension ref="B1:U47"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:I4"/>
+      <selection activeCell="G1" sqref="G1:M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -34660,10 +34866,10 @@
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:V48"/>
+  <dimension ref="B1:V48"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A2" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12:C16"/>
+    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1:M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -34675,6 +34881,14 @@
     <col min="12" max="12" width="12.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="2:22">
+      <c r="G1" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="K1" s="19" t="s">
+        <v>46</v>
+      </c>
+    </row>
     <row r="2" spans="2:22" ht="25">
       <c r="B2" s="4" t="s">
         <v>32</v>
@@ -34683,10 +34897,21 @@
         <f>D48+L48</f>
         <v>-4504.55</v>
       </c>
-      <c r="F2" t="s">
-        <v>35</v>
+      <c r="G2" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="I2" s="17">
+        <f>COUNTIF(D12:D42,"Y")/COUNT(C12:C42)</f>
+        <v>0.16129032258064516</v>
       </c>
       <c r="J2" s="1"/>
+      <c r="K2" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="M2" s="17">
+        <f>COUNTIF(L12:L42,"Y")/COUNT(K12:K42)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="3" spans="2:22" ht="25">
       <c r="B3" s="4" t="s">
@@ -34696,21 +34921,23 @@
         <f>C48+K48</f>
         <v>6091.73</v>
       </c>
-      <c r="F3" t="s">
-        <v>36</v>
+      <c r="G3" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="I3" s="18">
+        <f>AVERAGE(C12:C42)</f>
+        <v>143.12903225806451</v>
       </c>
       <c r="J3" s="1"/>
-      <c r="N3">
-        <v>6261.48</v>
-      </c>
-      <c r="O3" s="14">
-        <f>N3-D3</f>
-        <v>169.75</v>
-      </c>
-      <c r="Q3" s="14">
-        <f>O3+'September (2)'!O3</f>
-        <v>716.82999999999993</v>
-      </c>
+      <c r="K3" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="M3" s="18">
+        <f>AVERAGE(K12:K42)</f>
+        <v>224.90322580645162</v>
+      </c>
+      <c r="O3" s="14"/>
+      <c r="Q3" s="14"/>
     </row>
     <row r="4" spans="2:22" ht="25">
       <c r="B4" s="4" t="s">
@@ -34720,7 +34947,21 @@
         <f ca="1">D3-E44-M44</f>
         <v>-2471.2700000000004</v>
       </c>
+      <c r="G4" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="I4" s="18">
+        <f>I3*I2</f>
+        <v>23.085327783558792</v>
+      </c>
       <c r="J4" s="1"/>
+      <c r="K4" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="M4" s="18">
+        <f>M3*M2</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="5" spans="2:22">
       <c r="T5">
@@ -34731,9 +34972,6 @@
       </c>
     </row>
     <row r="6" spans="2:22">
-      <c r="F6" t="s">
-        <v>37</v>
-      </c>
       <c r="T6">
         <v>565.70399999999972</v>
       </c>
@@ -34742,9 +34980,6 @@
       </c>
     </row>
     <row r="7" spans="2:22">
-      <c r="F7" t="s">
-        <v>38</v>
-      </c>
       <c r="T7">
         <v>848.55600000000049</v>
       </c>
@@ -45915,10 +46150,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:U47"/>
+  <dimension ref="B1:U47"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -45930,6 +46165,14 @@
     <col min="12" max="12" width="12.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="2:21">
+      <c r="G1" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="K1" s="19" t="s">
+        <v>46</v>
+      </c>
+    </row>
     <row r="2" spans="2:21" ht="25">
       <c r="B2" s="4" t="s">
         <v>32</v>
@@ -45938,10 +46181,21 @@
         <f>D47+L47</f>
         <v>4216.33</v>
       </c>
-      <c r="F2" t="s">
-        <v>35</v>
+      <c r="G2" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="I2" s="17">
+        <f>COUNTIF(D12:D41,"Y")/COUNT(C12:C41)</f>
+        <v>0.8666666666666667</v>
       </c>
       <c r="J2" s="1"/>
+      <c r="K2" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="M2" s="17">
+        <f>COUNTIF(L12:L41,"Y")/COUNT(K12:K41)</f>
+        <v>0.6333333333333333</v>
+      </c>
     </row>
     <row r="3" spans="2:21" ht="25">
       <c r="B3" s="4" t="s">
@@ -45951,10 +46205,21 @@
         <f>C47+K47</f>
         <v>6238.78</v>
       </c>
-      <c r="F3" t="s">
-        <v>36</v>
+      <c r="G3" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="I3" s="18">
+        <f>AVERAGE(C12:C41)</f>
+        <v>157</v>
       </c>
       <c r="J3" s="1"/>
+      <c r="K3" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="M3" s="18">
+        <f>AVERAGE(K12:K41)</f>
+        <v>215.46666666666667</v>
+      </c>
     </row>
     <row r="4" spans="2:21" ht="25">
       <c r="B4" s="4" t="s">
@@ -45964,19 +46229,20 @@
         <f ca="1">D3-E43-M43</f>
         <v>4393.78</v>
       </c>
-      <c r="F4" t="s">
-        <v>57</v>
+      <c r="G4" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="I4" s="18">
+        <f>I3*I2</f>
+        <v>136.06666666666666</v>
       </c>
       <c r="J4" s="1"/>
-    </row>
-    <row r="6" spans="2:21">
-      <c r="F6" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="7" spans="2:21">
-      <c r="F7" t="s">
-        <v>38</v>
+      <c r="K4" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="M4" s="18">
+        <f>M3*M2</f>
+        <v>136.46222222222221</v>
       </c>
     </row>
     <row r="9" spans="2:21" ht="25">

</xml_diff>